<commit_message>
✨ Add busystations notebook
Finding the busiest stations by selecting the busiest times and then finding the stations with the most incoming bikes.  It is an aggregate so it doesn't make as much sense overall. :shrug:
</commit_message>
<xml_diff>
--- a/day_hour.xlsx
+++ b/day_hour.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/sql/bikeshare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716D472F-2CF9-3143-BBD7-DB9C558AA05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B803D9-9825-AE48-9648-510DBDF7B717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hourly" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="dayofweekextra" sheetId="5" r:id="rId3"/>
     <sheet name="month" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">hourly!$A$2:$B$169</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">hourly!$C$1</definedName>
@@ -35,66 +32,52 @@
     <definedName name="_xlchart.v1.18" hidden="1">hourly!$D$1</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">hourly!$D$2:$D$169</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">hourly!$C$2:$C$169</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">weekday!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">weekday!$B$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">weekday!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">weekday!$C$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">weekday!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">weekday!$D$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">weekday!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">weekday!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">weekday!$B$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">weekday!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">hourly!$A$2:$B$169</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">hourly!$F$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">hourly!$F$2:$F$169</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">hourly!$H$1</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">hourly!$H$2:$H$169</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">hourly!$A$2:$B$169</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">hourly!$C$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">hourly!$C$2:$C$169</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">hourly!$D$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">hourly!$D$2:$D$169</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">hourly!$D$1</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">weekday!$C$1</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">weekday!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">weekday!$D$1</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">weekday!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">weekday!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">weekday!$B$1</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">weekday!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">weekday!$C$1</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">weekday!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">weekday!$D$1</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">hourly!$A$2:$B$169</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">hourly!$C$1</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">hourly!$C$2:$C$169</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">hourly!$D$1</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">hourly!$D$2:$D$169</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">hourly!$A$2:$B$169</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">hourly!$C$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">hourly!$C$2:$C$169</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">hourly!$D$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">hourly!$D$2:$D$169</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">hourly!$D$2:$D$169</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">weekday!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">dayofweekextra!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">dayofweekextra!$E$1</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">dayofweekextra!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">dayofweekextra!$F$1</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">dayofweekextra!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">dayofweekextra!$G$1</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">dayofweekextra!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">dayofweekextra!$H$1</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">dayofweekextra!$H$2:$H$8</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">[1]sheet1!$A$2:$B$169</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">dayofweekextra!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">dayofweekextra!$E$1</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">dayofweekextra!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">dayofweekextra!$F$1</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">dayofweekextra!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">dayofweekextra!$G$1</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">dayofweekextra!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">dayofweekextra!$H$1</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">dayofweekextra!$H$2:$H$8</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">month!$A$2:$A$13</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">[1]sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">month!$B$1</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">month!$B$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">month!$C$1</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">month!$C$2:$C$13</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">month!$E$1</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">month!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">month!$A$2:$A$13</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">month!$B$1</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">month!$B$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">month!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">[1]sheet1!$C$2:$C$169</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">month!$C$2:$C$13</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">month!$E$1</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">month!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">[1]sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">[1]sheet1!$D$2:$D$169</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">hourly!$A$2:$B$169</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">hourly!$C$1</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">hourly!$C$2:$C$169</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">hourly!$D$1</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">hourly!$D$2:$D$169</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">weekday!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">weekday!$B$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">weekday!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">weekday!$C$1</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">weekday!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">hourly!$A$2:$B$169</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">weekday!$D$1</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">weekday!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">weekday!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">weekday!$B$1</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">weekday!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">weekday!$C$1</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">weekday!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">weekday!$D$1</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">weekday!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">hourly!$C$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">hourly!$C$2:$C$169</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">hourly!$D$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">hourly!$D$2:$D$169</definedName>
     <definedName name="month" localSheetId="3">month!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -118,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t>day</t>
   </si>
@@ -305,33 +288,100 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2800" b="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+                <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t>2018-19 Ridership Change</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2800" b="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+                <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2800" b="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+                <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t>by Time of Day / Day of Week</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12395301301623013"/>
+          <c:y val="9.5728597221525644E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:alpha val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="38100" h="38100"/>
+        </a:sp3d>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -344,7 +394,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.9917660292463441E-2"/>
+          <c:y val="5.1716234515271575E-2"/>
+          <c:w val="0.94911380363168885"/>
+          <c:h val="0.85720973970610359"/>
+        </c:manualLayout>
+      </c:layout>
       <c:areaChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -364,12 +424,29 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="9525">
               <a:noFill/>
+              <a:prstDash val="solid"/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" algn="l" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="plastic">
+              <a:bevelT prst="angle"/>
+            </a:sp3d>
           </c:spPr>
           <c:cat>
             <c:multiLvlStrRef>
@@ -1025,13 +1102,27 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="152400" h="50800" prst="softRound"/>
+            </a:sp3d>
           </c:spPr>
           <c:cat>
             <c:multiLvlStrRef>
@@ -1714,10 +1805,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1732,6 +1820,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="6"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -1788,10 +1877,20 @@
         </c:txPr>
         <c:crossAx val="1693670367"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:pattFill prst="narVert">
+          <a:fgClr>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="bg1"/>
+          </a:bgClr>
+        </a:pattFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1800,20 +1899,38 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76728330387273025"/>
+          <c:y val="0.29960955915542403"/>
+          <c:w val="0.16146861642294713"/>
+          <c:h val="3.6495185315211398E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw blurRad="76200" dir="18900000" sx="101000" sy="101000" kx="-1200000" algn="bl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="51000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
       </c:spPr>
       <c:txPr>
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1841,9 +1958,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -1887,41 +2002,21 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.421907627944323E-2"/>
+          <c:y val="2.8012440170280345E-2"/>
+          <c:w val="0.89680708196895964"/>
+          <c:h val="0.73353919903537212"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1938,9 +2033,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1955,27 +2050,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="38100" cap="rnd">
-                <a:solidFill>
-                  <a:srgbClr val="C00000"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="6"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:multiLvlStrRef>
               <c:f>hourly!$A$2:$B$169</c:f>
               <c:multiLvlStrCache>
@@ -2094,520 +2169,187 @@
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>hourly!$F$2:$F$169</c:f>
+              <c:f>hourly!$G$2:$G$169</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="168"/>
                 <c:pt idx="0">
                   <c:v>0.35899999999999999</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.3866</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.58520000000000005</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>0.29020000000000001</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.59079999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.3871</c:v>
-                </c:pt>
                 <c:pt idx="6">
                   <c:v>0.40100000000000002</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.39810000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.40300000000000002</c:v>
-                </c:pt>
                 <c:pt idx="9">
                   <c:v>0.49049999999999999</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.51619999999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.51839999999999997</c:v>
-                </c:pt>
                 <c:pt idx="12">
                   <c:v>0.4773</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.45950000000000002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.52290000000000003</c:v>
-                </c:pt>
                 <c:pt idx="15">
                   <c:v>0.44679999999999997</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.43569999999999998</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.42899999999999999</c:v>
-                </c:pt>
                 <c:pt idx="18">
                   <c:v>0.48010000000000003</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.49020000000000002</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.49640000000000001</c:v>
-                </c:pt>
                 <c:pt idx="21">
                   <c:v>0.48530000000000001</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.44890000000000002</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.4123</c:v>
-                </c:pt>
                 <c:pt idx="24">
                   <c:v>0.39400000000000002</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.45129999999999998</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.53669999999999995</c:v>
-                </c:pt>
                 <c:pt idx="27">
                   <c:v>0.96730000000000005</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.53700000000000003</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.41199999999999998</c:v>
-                </c:pt>
                 <c:pt idx="30">
                   <c:v>0.32490000000000002</c:v>
                 </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.31259999999999999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.35020000000000001</c:v>
-                </c:pt>
                 <c:pt idx="33">
                   <c:v>0.41370000000000001</c:v>
                 </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.44259999999999999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.44290000000000002</c:v>
-                </c:pt>
                 <c:pt idx="36">
                   <c:v>0.43880000000000002</c:v>
                 </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.46729999999999999</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.50780000000000003</c:v>
-                </c:pt>
                 <c:pt idx="39">
                   <c:v>0.53790000000000004</c:v>
                 </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.48280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.50829999999999997</c:v>
-                </c:pt>
                 <c:pt idx="42">
                   <c:v>0.51900000000000002</c:v>
                 </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.54379999999999995</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.45660000000000001</c:v>
-                </c:pt>
                 <c:pt idx="45">
                   <c:v>0.45300000000000001</c:v>
                 </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.4194</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.49030000000000001</c:v>
-                </c:pt>
                 <c:pt idx="48">
                   <c:v>0.27589999999999998</c:v>
                 </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.36499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.54149999999999998</c:v>
-                </c:pt>
                 <c:pt idx="51">
                   <c:v>0.1353</c:v>
                 </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.30620000000000003</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.4244</c:v>
-                </c:pt>
                 <c:pt idx="54">
                   <c:v>0.3785</c:v>
                 </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.35709999999999997</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.39450000000000002</c:v>
-                </c:pt>
                 <c:pt idx="57">
                   <c:v>0.43149999999999999</c:v>
                 </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.35859999999999997</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.37080000000000002</c:v>
-                </c:pt>
                 <c:pt idx="60">
                   <c:v>0.32890000000000003</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.35360000000000003</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.42180000000000001</c:v>
-                </c:pt>
                 <c:pt idx="63">
                   <c:v>0.42909999999999998</c:v>
                 </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.30909999999999999</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.28770000000000001</c:v>
-                </c:pt>
                 <c:pt idx="66">
                   <c:v>0.33360000000000001</c:v>
                 </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.34350000000000003</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.3473</c:v>
-                </c:pt>
                 <c:pt idx="69">
                   <c:v>0.2984</c:v>
                 </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.33100000000000002</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.1293</c:v>
-                </c:pt>
                 <c:pt idx="72">
                   <c:v>0.24360000000000001</c:v>
                 </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.39279999999999998</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.34720000000000001</c:v>
-                </c:pt>
                 <c:pt idx="75">
                   <c:v>0.3029</c:v>
                 </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.34720000000000001</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.44159999999999999</c:v>
-                </c:pt>
                 <c:pt idx="78">
                   <c:v>0.28560000000000002</c:v>
                 </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.29659999999999997</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.27529999999999999</c:v>
-                </c:pt>
                 <c:pt idx="81">
                   <c:v>0.35110000000000002</c:v>
                 </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.35670000000000002</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.31909999999999999</c:v>
-                </c:pt>
                 <c:pt idx="84">
                   <c:v>0.28270000000000001</c:v>
                 </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.34410000000000002</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.38300000000000001</c:v>
-                </c:pt>
                 <c:pt idx="87">
                   <c:v>0.42409999999999998</c:v>
                 </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.41660000000000003</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.37090000000000001</c:v>
-                </c:pt>
                 <c:pt idx="90">
                   <c:v>0.39939999999999998</c:v>
                 </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.41349999999999998</c:v>
-                </c:pt>
                 <c:pt idx="93">
                   <c:v>0.496</c:v>
                 </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.39500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.64770000000000005</c:v>
-                </c:pt>
                 <c:pt idx="96">
                   <c:v>0.41930000000000001</c:v>
                 </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.52139999999999997</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.52659999999999996</c:v>
-                </c:pt>
                 <c:pt idx="99">
                   <c:v>0.4627</c:v>
                 </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.48620000000000002</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.34110000000000001</c:v>
-                </c:pt>
                 <c:pt idx="102">
                   <c:v>0.28029999999999999</c:v>
                 </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.3417</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.39879999999999999</c:v>
-                </c:pt>
                 <c:pt idx="105">
                   <c:v>0.42549999999999999</c:v>
                 </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.40699999999999997</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.43559999999999999</c:v>
-                </c:pt>
                 <c:pt idx="108">
                   <c:v>0.4052</c:v>
                 </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.40699999999999997</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.37009999999999998</c:v>
-                </c:pt>
                 <c:pt idx="111">
                   <c:v>0.38740000000000002</c:v>
                 </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.30120000000000002</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.38150000000000001</c:v>
-                </c:pt>
                 <c:pt idx="114">
                   <c:v>0.45679999999999998</c:v>
                 </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.47389999999999999</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.48830000000000001</c:v>
-                </c:pt>
                 <c:pt idx="117">
                   <c:v>0.40620000000000001</c:v>
                 </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.40960000000000002</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.3518</c:v>
-                </c:pt>
                 <c:pt idx="120">
                   <c:v>0.44519999999999998</c:v>
                 </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.4909</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.3538</c:v>
-                </c:pt>
                 <c:pt idx="123">
                   <c:v>0.36009999999999998</c:v>
                 </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.248</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.58420000000000005</c:v>
-                </c:pt>
                 <c:pt idx="126">
                   <c:v>0.42730000000000001</c:v>
                 </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.35039999999999999</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>0.40960000000000002</c:v>
-                </c:pt>
                 <c:pt idx="129">
                   <c:v>0.46200000000000002</c:v>
                 </c:pt>
-                <c:pt idx="130">
-                  <c:v>0.44540000000000002</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>0.54139999999999999</c:v>
-                </c:pt>
                 <c:pt idx="132">
                   <c:v>0.59419999999999995</c:v>
                 </c:pt>
-                <c:pt idx="133">
-                  <c:v>0.54600000000000004</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>0.56430000000000002</c:v>
-                </c:pt>
                 <c:pt idx="135">
                   <c:v>0.58169999999999999</c:v>
                 </c:pt>
-                <c:pt idx="136">
-                  <c:v>0.53639999999999999</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>0.55110000000000003</c:v>
-                </c:pt>
                 <c:pt idx="138">
                   <c:v>0.5595</c:v>
                 </c:pt>
-                <c:pt idx="139">
-                  <c:v>0.54059999999999997</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>0.52</c:v>
-                </c:pt>
                 <c:pt idx="141">
                   <c:v>0.58260000000000001</c:v>
                 </c:pt>
-                <c:pt idx="142">
-                  <c:v>0.53080000000000005</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>0.55469999999999997</c:v>
-                </c:pt>
                 <c:pt idx="144">
                   <c:v>0.58389999999999997</c:v>
                 </c:pt>
-                <c:pt idx="145">
-                  <c:v>0.70230000000000004</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>0.52080000000000004</c:v>
-                </c:pt>
                 <c:pt idx="147">
                   <c:v>0.38879999999999998</c:v>
                 </c:pt>
-                <c:pt idx="148">
-                  <c:v>0.73129999999999995</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>0.74819999999999998</c:v>
-                </c:pt>
                 <c:pt idx="150">
                   <c:v>0.68389999999999995</c:v>
                 </c:pt>
-                <c:pt idx="151">
-                  <c:v>0.56489999999999996</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>0.58420000000000005</c:v>
-                </c:pt>
                 <c:pt idx="153">
                   <c:v>0.57940000000000003</c:v>
                 </c:pt>
-                <c:pt idx="154">
-                  <c:v>0.51719999999999999</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>0.50290000000000001</c:v>
-                </c:pt>
                 <c:pt idx="156">
                   <c:v>0.45829999999999999</c:v>
                 </c:pt>
-                <c:pt idx="157">
-                  <c:v>0.4531</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>0.42930000000000001</c:v>
-                </c:pt>
                 <c:pt idx="159">
                   <c:v>0.40560000000000002</c:v>
                 </c:pt>
-                <c:pt idx="160">
-                  <c:v>0.46550000000000002</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>0.4723</c:v>
-                </c:pt>
                 <c:pt idx="162">
                   <c:v>0.51100000000000001</c:v>
                 </c:pt>
-                <c:pt idx="163">
-                  <c:v>0.4743</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>0.59989999999999999</c:v>
-                </c:pt>
                 <c:pt idx="165">
                   <c:v>0.53869999999999996</c:v>
                 </c:pt>
-                <c:pt idx="166">
-                  <c:v>0.62380000000000002</c:v>
-                </c:pt>
                 <c:pt idx="167">
                   <c:v>0.50039999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2623,11 +2365,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="1693670367"/>
         <c:axId val="1693966639"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1693670367"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -2673,11 +2414,8 @@
         </c:txPr>
         <c:crossAx val="1693966639"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1693966639"/>
         <c:scaling>
@@ -2686,20 +2424,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2733,7 +2457,7 @@
         </c:txPr>
         <c:crossAx val="1693670367"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2743,8 +2467,39 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="span"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -5647,41 +5402,28 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
   <cs:variation>
-    <a:lumMod val="60000"/>
+    <a:tint val="88500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
+    <a:tint val="55000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
+    <a:tint val="75000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
+    <a:tint val="98500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50000"/>
+    <a:tint val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
+    <a:tint val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
+    <a:tint val="80000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
@@ -9518,16 +9260,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>97972</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>16329</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>89506</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>720272</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>79829</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>711806</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>160866</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9554,16 +9296,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>90714</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>90714</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>56849</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>107647</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>713014</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>154214</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>584201</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9790,19 +9532,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10106,15 +9835,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F169"/>
+  <dimension ref="A1:J169"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="Z39" sqref="Z39"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10133,8 +9868,20 @@
       <c r="F1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -10153,8 +9900,20 @@
       <c r="F2" s="2">
         <v>0.35899999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G2" s="2">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.27410000000000001</v>
+      </c>
+      <c r="J2" s="2">
+        <v>-0.18790000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" s="1">
         <v>882</v>
       </c>
@@ -10167,8 +9926,16 @@
       <c r="F3" s="2">
         <v>0.3866</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G3" s="2"/>
+      <c r="H3" s="1">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
+        <v>-0.12540000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="1">
         <v>446</v>
       </c>
@@ -10181,8 +9948,16 @@
       <c r="F4" s="2">
         <v>0.58520000000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G4" s="2"/>
+      <c r="H4" s="1">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
+        <v>0.32390000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="1">
         <v>224</v>
       </c>
@@ -10195,8 +9970,20 @@
       <c r="F5" s="2">
         <v>0.29020000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G5" s="2">
+        <v>0.29020000000000001</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.192</v>
+      </c>
+      <c r="J5" s="2">
+        <v>-0.34350000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="1">
         <v>347</v>
       </c>
@@ -10209,8 +9996,16 @@
       <c r="F6" s="2">
         <v>0.59079999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G6" s="2"/>
+      <c r="H6" s="1">
+        <v>1.03E-2</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
+        <v>0.33650000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="1">
         <v>1860</v>
       </c>
@@ -10223,8 +10018,16 @@
       <c r="F7" s="2">
         <v>0.3871</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G7" s="2"/>
+      <c r="H7" s="1">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
+        <v>-0.12429999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -10240,8 +10043,20 @@
       <c r="F8" s="2">
         <v>0.40100000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G8" s="2">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.1389</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.32419999999999999</v>
+      </c>
+      <c r="J8" s="2">
+        <v>-9.2899999999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" s="1">
         <v>16947</v>
       </c>
@@ -10254,8 +10069,16 @@
       <c r="F9" s="2">
         <v>0.39810000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G9" s="2"/>
+      <c r="H9" s="1">
+        <v>0.39119999999999999</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
+        <v>-9.9500000000000005E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" s="1">
         <v>29106</v>
       </c>
@@ -10268,8 +10091,16 @@
       <c r="F10" s="2">
         <v>0.40300000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G10" s="2"/>
+      <c r="H10" s="1">
+        <v>0.68140000000000001</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2">
+        <v>-8.8400000000000006E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" s="1">
         <v>14872</v>
       </c>
@@ -10282,8 +10113,20 @@
       <c r="F11" s="2">
         <v>0.49049999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G11" s="2">
+        <v>0.49049999999999999</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.42320000000000002</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.43109999999999998</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.10970000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="1">
         <v>9116</v>
       </c>
@@ -10296,8 +10139,16 @@
       <c r="F12" s="2">
         <v>0.51619999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G12" s="2"/>
+      <c r="H12" s="1">
+        <v>0.27239999999999998</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
+        <v>0.16789999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" s="1">
         <v>9635</v>
       </c>
@@ -10310,8 +10161,16 @@
       <c r="F13" s="2">
         <v>0.51839999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G13" s="2"/>
+      <c r="H13" s="1">
+        <v>0.28920000000000001</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <v>0.17280000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -10327,8 +10186,20 @@
       <c r="F14" s="2">
         <v>0.4773</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G14" s="2">
+        <v>0.4773</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.318</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.4153</v>
+      </c>
+      <c r="J14" s="2">
+        <v>7.9799999999999996E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" s="1">
         <v>10984</v>
       </c>
@@ -10341,8 +10212,16 @@
       <c r="F15" s="2">
         <v>0.45950000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G15" s="2"/>
+      <c r="H15" s="1">
+        <v>0.2923</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2">
+        <v>3.95E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" s="1">
         <v>10774</v>
       </c>
@@ -10355,8 +10234,16 @@
       <c r="F16" s="2">
         <v>0.52290000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G16" s="2"/>
+      <c r="H16" s="1">
+        <v>0.32650000000000001</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C17" s="1">
         <v>13406</v>
       </c>
@@ -10369,8 +10256,20 @@
       <c r="F17" s="2">
         <v>0.44679999999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G17" s="2">
+        <v>0.44679999999999997</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.34720000000000001</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.37890000000000001</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1.0800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C18" s="1">
         <v>22574</v>
       </c>
@@ -10383,8 +10282,16 @@
       <c r="F18" s="2">
         <v>0.43569999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G18" s="2"/>
+      <c r="H18" s="1">
+        <v>0.57110000000000005</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2">
+        <v>-1.44E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C19" s="1">
         <v>33529</v>
       </c>
@@ -10397,8 +10304,16 @@
       <c r="F19" s="2">
         <v>0.42899999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G19" s="2"/>
+      <c r="H19" s="1">
+        <v>0.83609999999999995</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2">
+        <v>-2.9399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -10414,8 +10329,20 @@
       <c r="F20" s="2">
         <v>0.48010000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G20" s="2">
+        <v>0.48010000000000003</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.64639999999999997</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.41860000000000003</v>
+      </c>
+      <c r="J20" s="2">
+        <v>8.6099999999999996E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C21" s="1">
         <v>15289</v>
       </c>
@@ -10428,8 +10355,16 @@
       <c r="F21" s="2">
         <v>0.49020000000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G21" s="2"/>
+      <c r="H21" s="1">
+        <v>0.43480000000000002</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C22" s="1">
         <v>10078</v>
       </c>
@@ -10442,8 +10377,16 @@
       <c r="F22" s="2">
         <v>0.49640000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G22" s="2"/>
+      <c r="H22" s="1">
+        <v>0.28970000000000001</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2">
+        <v>0.1231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C23" s="1">
         <v>6854</v>
       </c>
@@ -10456,8 +10399,20 @@
       <c r="F23" s="2">
         <v>0.48530000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G23" s="2">
+        <v>0.48530000000000001</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.19209999999999999</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.42480000000000001</v>
+      </c>
+      <c r="J23" s="2">
+        <v>9.7799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C24" s="1">
         <v>4440</v>
       </c>
@@ -10470,8 +10425,16 @@
       <c r="F24" s="2">
         <v>0.44890000000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G24" s="2"/>
+      <c r="H24" s="1">
+        <v>0.1144</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2">
+        <v>1.55E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C25" s="1">
         <v>2401</v>
       </c>
@@ -10484,8 +10447,16 @@
       <c r="F25" s="2">
         <v>0.4123</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G25" s="2"/>
+      <c r="H25" s="1">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2">
+        <v>-6.7199999999999996E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -10504,8 +10475,20 @@
       <c r="F26" s="2">
         <v>0.39400000000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G26" s="2">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2.53E-2</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.31590000000000001</v>
+      </c>
+      <c r="J26" s="2">
+        <v>-0.1086</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C27" s="1">
         <v>585</v>
       </c>
@@ -10518,8 +10501,16 @@
       <c r="F27" s="2">
         <v>0.45129999999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G27" s="2"/>
+      <c r="H27" s="1">
+        <v>1.37E-2</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2">
+        <v>2.0899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C28" s="1">
         <v>354</v>
       </c>
@@ -10532,8 +10523,16 @@
       <c r="F28" s="2">
         <v>0.53669999999999995</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G28" s="2"/>
+      <c r="H28" s="1">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2">
+        <v>0.2142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C29" s="1">
         <v>153</v>
       </c>
@@ -10546,8 +10545,20 @@
       <c r="F29" s="2">
         <v>0.96730000000000005</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G29" s="2">
+        <v>0.96730000000000005</v>
+      </c>
+      <c r="H29" s="1">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1.1882999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C30" s="1">
         <v>324</v>
       </c>
@@ -10560,8 +10571,16 @@
       <c r="F30" s="2">
         <v>0.53700000000000003</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G30" s="2"/>
+      <c r="H30" s="1">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2">
+        <v>0.21490000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C31" s="1">
         <v>2090</v>
       </c>
@@ -10574,8 +10593,16 @@
       <c r="F31" s="2">
         <v>0.41199999999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G31" s="2"/>
+      <c r="H31" s="1">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2">
+        <v>-6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>8</v>
       </c>
@@ -10591,8 +10618,20 @@
       <c r="F32" s="2">
         <v>0.32490000000000002</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G32" s="2">
+        <v>0.32490000000000002</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0.2334</v>
+      </c>
+      <c r="J32" s="2">
+        <v>-0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C33" s="1">
         <v>19600</v>
       </c>
@@ -10605,8 +10644,16 @@
       <c r="F33" s="2">
         <v>0.31259999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G33" s="2"/>
+      <c r="H33" s="1">
+        <v>0.35510000000000003</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2">
+        <v>-0.29289999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C34" s="1">
         <v>32890</v>
       </c>
@@ -10619,8 +10666,16 @@
       <c r="F34" s="2">
         <v>0.35020000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G34" s="2"/>
+      <c r="H34" s="1">
+        <v>0.66910000000000003</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2">
+        <v>-0.20780000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C35" s="1">
         <v>16363</v>
       </c>
@@ -10633,8 +10688,20 @@
       <c r="F35" s="2">
         <v>0.41370000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G35" s="2">
+        <v>0.41370000000000001</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.3926</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0.33939999999999998</v>
+      </c>
+      <c r="J35" s="2">
+        <v>-6.4100000000000004E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C36" s="1">
         <v>9063</v>
       </c>
@@ -10647,8 +10714,16 @@
       <c r="F36" s="2">
         <v>0.44259999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G36" s="2"/>
+      <c r="H36" s="1">
+        <v>0.2319</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C37" s="1">
         <v>9359</v>
       </c>
@@ -10661,8 +10736,16 @@
       <c r="F37" s="2">
         <v>0.44290000000000002</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G37" s="2"/>
+      <c r="H37" s="1">
+        <v>0.23980000000000001</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2">
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>9</v>
       </c>
@@ -10678,8 +10761,20 @@
       <c r="F38" s="2">
         <v>0.43880000000000002</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G38" s="2">
+        <v>0.43880000000000002</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.27660000000000001</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0.36930000000000002</v>
+      </c>
+      <c r="J38" s="2">
+        <v>-7.3000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C39" s="1">
         <v>10147</v>
       </c>
@@ -10692,8 +10787,16 @@
       <c r="F39" s="2">
         <v>0.46729999999999999</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G39" s="2"/>
+      <c r="H39" s="1">
+        <v>0.27450000000000002</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2">
+        <v>5.7200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C40" s="1">
         <v>9816</v>
       </c>
@@ -10706,8 +10809,16 @@
       <c r="F40" s="2">
         <v>0.50780000000000003</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G40" s="2"/>
+      <c r="H40" s="1">
+        <v>0.28870000000000001</v>
+      </c>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2">
+        <v>0.1489</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C41" s="1">
         <v>12016</v>
       </c>
@@ -10720,8 +10831,20 @@
       <c r="F41" s="2">
         <v>0.53790000000000004</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G41" s="2">
+        <v>0.53790000000000004</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.37469999999999998</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0.48759999999999998</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0.21679999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C42" s="1">
         <v>22270</v>
       </c>
@@ -10734,8 +10857,16 @@
       <c r="F42" s="2">
         <v>0.48280000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G42" s="2"/>
+      <c r="H42" s="1">
+        <v>0.62460000000000004</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2">
+        <v>9.2299999999999993E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C43" s="1">
         <v>33838</v>
       </c>
@@ -10748,8 +10879,16 @@
       <c r="F43" s="2">
         <v>0.50829999999999997</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G43" s="2"/>
+      <c r="H43" s="1">
+        <v>1</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2">
+        <v>0.14990000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>10</v>
       </c>
@@ -10765,8 +10904,20 @@
       <c r="F44" s="2">
         <v>0.51900000000000002</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G44" s="2">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.73280000000000001</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0.1741</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C45" s="1">
         <v>15609</v>
       </c>
@@ -10779,8 +10930,16 @@
       <c r="F45" s="2">
         <v>0.54379999999999995</v>
       </c>
-    </row>
-    <row r="46" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G45" s="2"/>
+      <c r="H45" s="1">
+        <v>0.49270000000000003</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2">
+        <v>0.23019999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C46" s="1">
         <v>10967</v>
       </c>
@@ -10793,8 +10952,16 @@
       <c r="F46" s="2">
         <v>0.45660000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G46" s="2"/>
+      <c r="H46" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2">
+        <v>3.3099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C47" s="1">
         <v>8002</v>
       </c>
@@ -10807,8 +10974,20 @@
       <c r="F47" s="2">
         <v>0.45300000000000001</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G47" s="2">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.20949999999999999</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0.38629999999999998</v>
+      </c>
+      <c r="J47" s="2">
+        <v>2.4799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C48" s="1">
         <v>5453</v>
       </c>
@@ -10821,8 +11000,16 @@
       <c r="F48" s="2">
         <v>0.4194</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G48" s="2"/>
+      <c r="H48" s="1">
+        <v>0.13159999999999999</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2">
+        <v>-5.1200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C49" s="1">
         <v>2835</v>
       </c>
@@ -10835,8 +11022,16 @@
       <c r="F49" s="2">
         <v>0.49030000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G49" s="2"/>
+      <c r="H49" s="1">
+        <v>7.9299999999999995E-2</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2">
+        <v>0.10920000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -10855,8 +11050,20 @@
       <c r="F50" s="2">
         <v>0.27589999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G50" s="2">
+        <v>0.27589999999999998</v>
+      </c>
+      <c r="H50" s="1">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0.1749</v>
+      </c>
+      <c r="J50" s="2">
+        <v>-0.37590000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C51" s="1">
         <v>737</v>
       </c>
@@ -10869,8 +11076,16 @@
       <c r="F51" s="2">
         <v>0.36499999999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G51" s="2"/>
+      <c r="H51" s="1">
+        <v>1.4E-2</v>
+      </c>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2">
+        <v>-0.17430000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C52" s="1">
         <v>386</v>
       </c>
@@ -10883,8 +11098,16 @@
       <c r="F52" s="2">
         <v>0.54149999999999998</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G52" s="2"/>
+      <c r="H52" s="1">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2">
+        <v>0.22489999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C53" s="1">
         <v>207</v>
       </c>
@@ -10897,8 +11120,20 @@
       <c r="F53" s="2">
         <v>0.1353</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G53" s="2">
+        <v>0.1353</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="J53" s="2">
+        <v>-0.69399999999999995</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C54" s="1">
         <v>369</v>
       </c>
@@ -10911,8 +11146,16 @@
       <c r="F54" s="2">
         <v>0.30620000000000003</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G54" s="2"/>
+      <c r="H54" s="1">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2">
+        <v>-0.30719999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C55" s="1">
         <v>2144</v>
       </c>
@@ -10925,8 +11168,16 @@
       <c r="F55" s="2">
         <v>0.4244</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G55" s="2"/>
+      <c r="H55" s="1">
+        <v>5.1400000000000001E-2</v>
+      </c>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2">
+        <v>-3.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>8</v>
       </c>
@@ -10942,8 +11193,20 @@
       <c r="F56" s="2">
         <v>0.3785</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G56" s="2">
+        <v>0.3785</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0.15590000000000001</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0.2974</v>
+      </c>
+      <c r="J56" s="2">
+        <v>-0.14369999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C57" s="1">
         <v>20036</v>
       </c>
@@ -10956,8 +11219,16 @@
       <c r="F57" s="2">
         <v>0.35709999999999997</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G57" s="2"/>
+      <c r="H57" s="1">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2">
+        <v>-0.19220000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C58" s="1">
         <v>33162</v>
       </c>
@@ -10970,8 +11241,16 @@
       <c r="F58" s="2">
         <v>0.39450000000000002</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G58" s="2"/>
+      <c r="H58" s="1">
+        <v>0.76019999999999999</v>
+      </c>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2">
+        <v>-0.1075</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C59" s="1">
         <v>17197</v>
       </c>
@@ -10984,8 +11263,20 @@
       <c r="F59" s="2">
         <v>0.43149999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G59" s="2">
+        <v>0.43149999999999999</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0.43049999999999999</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0.36070000000000002</v>
+      </c>
+      <c r="J59" s="2">
+        <v>-2.3800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C60" s="1">
         <v>10189</v>
       </c>
@@ -10998,8 +11289,16 @@
       <c r="F60" s="2">
         <v>0.35859999999999997</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G60" s="2"/>
+      <c r="H60" s="1">
+        <v>0.2112</v>
+      </c>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2">
+        <v>-0.18870000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C61" s="1">
         <v>10582</v>
       </c>
@@ -11012,8 +11311,16 @@
       <c r="F61" s="2">
         <v>0.37080000000000002</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G61" s="2"/>
+      <c r="H61" s="1">
+        <v>0.22689999999999999</v>
+      </c>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2">
+        <v>-0.16109999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>9</v>
       </c>
@@ -11029,8 +11336,20 @@
       <c r="F62" s="2">
         <v>0.32890000000000003</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G62" s="2">
+        <v>0.32890000000000003</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0.2384</v>
+      </c>
+      <c r="I62" s="2">
+        <v>0.2382</v>
+      </c>
+      <c r="J62" s="2">
+        <v>-0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C63" s="1">
         <v>11723</v>
       </c>
@@ -11043,8 +11362,16 @@
       <c r="F63" s="2">
         <v>0.35360000000000003</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G63" s="2"/>
+      <c r="H63" s="1">
+        <v>0.23980000000000001</v>
+      </c>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2">
+        <v>-0.2001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C64" s="1">
         <v>11097</v>
       </c>
@@ -11057,8 +11384,16 @@
       <c r="F64" s="2">
         <v>0.42180000000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G64" s="2"/>
+      <c r="H64" s="1">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2">
+        <v>-4.5699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C65" s="1">
         <v>13604</v>
       </c>
@@ -11071,8 +11406,20 @@
       <c r="F65" s="2">
         <v>0.42909999999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G65" s="2">
+        <v>0.42909999999999998</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0.33829999999999999</v>
+      </c>
+      <c r="I65" s="2">
+        <v>0.35770000000000002</v>
+      </c>
+      <c r="J65" s="2">
+        <v>-2.93E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C66" s="1">
         <v>24554</v>
       </c>
@@ -11085,8 +11432,16 @@
       <c r="F66" s="2">
         <v>0.30909999999999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G66" s="2"/>
+      <c r="H66" s="1">
+        <v>0.44030000000000002</v>
+      </c>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2">
+        <v>-0.30080000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C67" s="1">
         <v>37229</v>
       </c>
@@ -11099,8 +11454,16 @@
       <c r="F67" s="2">
         <v>0.28770000000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G67" s="2"/>
+      <c r="H67" s="1">
+        <v>0.622</v>
+      </c>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2">
+        <v>-0.3493</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>10</v>
       </c>
@@ -11116,8 +11479,20 @@
       <c r="F68" s="2">
         <v>0.33360000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G68" s="2">
+        <v>0.33360000000000001</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0.50529999999999997</v>
+      </c>
+      <c r="I68" s="2">
+        <v>0.24379999999999999</v>
+      </c>
+      <c r="J68" s="2">
+        <v>-0.24540000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C69" s="1">
         <v>17850</v>
       </c>
@@ -11130,8 +11505,16 @@
       <c r="F69" s="2">
         <v>0.34350000000000003</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G69" s="2"/>
+      <c r="H69" s="1">
+        <v>0.35549999999999998</v>
+      </c>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2">
+        <v>-0.2228</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C70" s="1">
         <v>11862</v>
       </c>
@@ -11144,8 +11527,16 @@
       <c r="F70" s="2">
         <v>0.3473</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G70" s="2"/>
+      <c r="H70" s="1">
+        <v>0.23830000000000001</v>
+      </c>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2">
+        <v>-0.2142</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C71" s="1">
         <v>8809</v>
       </c>
@@ -11158,8 +11549,20 @@
       <c r="F71" s="2">
         <v>0.2984</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G71" s="2">
+        <v>0.2984</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0.1515</v>
+      </c>
+      <c r="I71" s="2">
+        <v>0.2019</v>
+      </c>
+      <c r="J71" s="2">
+        <v>-0.32479999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C72" s="1">
         <v>5782</v>
       </c>
@@ -11172,8 +11575,16 @@
       <c r="F72" s="2">
         <v>0.33100000000000002</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G72" s="2"/>
+      <c r="H72" s="1">
+        <v>0.10979999999999999</v>
+      </c>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2">
+        <v>-0.25109999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C73" s="1">
         <v>3744</v>
       </c>
@@ -11186,8 +11597,16 @@
       <c r="F73" s="2">
         <v>0.1293</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G73" s="2"/>
+      <c r="H73" s="1">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2">
+        <v>-0.70750000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -11206,8 +11625,20 @@
       <c r="F74" s="2">
         <v>0.24360000000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G74" s="2">
+        <v>0.24360000000000001</v>
+      </c>
+      <c r="H74" s="1">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="I74" s="2">
+        <v>0.13650000000000001</v>
+      </c>
+      <c r="J74" s="2">
+        <v>-0.44879999999999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C75" s="1">
         <v>779</v>
       </c>
@@ -11220,8 +11651,16 @@
       <c r="F75" s="2">
         <v>0.39279999999999998</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G75" s="2"/>
+      <c r="H75" s="1">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2">
+        <v>-0.1114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C76" s="1">
         <v>458</v>
       </c>
@@ -11234,8 +11673,16 @@
       <c r="F76" s="2">
         <v>0.34720000000000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G76" s="2"/>
+      <c r="H76" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2">
+        <v>-0.21460000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C77" s="1">
         <v>208</v>
       </c>
@@ -11248,8 +11695,20 @@
       <c r="F77" s="2">
         <v>0.3029</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G77" s="2">
+        <v>0.3029</v>
+      </c>
+      <c r="H77" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="I77" s="2">
+        <v>0.2072</v>
+      </c>
+      <c r="J77" s="2">
+        <v>-0.31480000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C78" s="1">
         <v>337</v>
       </c>
@@ -11262,8 +11721,16 @@
       <c r="F78" s="2">
         <v>0.34720000000000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G78" s="2"/>
+      <c r="H78" s="1">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2">
+        <v>-0.21460000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C79" s="1">
         <v>1866</v>
       </c>
@@ -11276,8 +11743,16 @@
       <c r="F79" s="2">
         <v>0.44159999999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G79" s="2"/>
+      <c r="H79" s="1">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2">
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>8</v>
       </c>
@@ -11293,8 +11768,20 @@
       <c r="F80" s="2">
         <v>0.28560000000000002</v>
       </c>
-    </row>
-    <row r="81" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G80" s="2">
+        <v>0.28560000000000002</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0.1118</v>
+      </c>
+      <c r="I80" s="2">
+        <v>0.1865</v>
+      </c>
+      <c r="J80" s="2">
+        <v>-0.35389999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C81" s="1">
         <v>18982</v>
       </c>
@@ -11307,8 +11794,16 @@
       <c r="F81" s="2">
         <v>0.29659999999999997</v>
       </c>
-    </row>
-    <row r="82" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G81" s="2"/>
+      <c r="H81" s="1">
+        <v>0.32629999999999998</v>
+      </c>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2">
+        <v>-0.32890000000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C82" s="1">
         <v>33130</v>
       </c>
@@ -11321,8 +11816,16 @@
       <c r="F82" s="2">
         <v>0.27529999999999999</v>
       </c>
-    </row>
-    <row r="83" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G82" s="2"/>
+      <c r="H82" s="1">
+        <v>0.52949999999999997</v>
+      </c>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2">
+        <v>-0.37719999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C83" s="1">
         <v>17252</v>
       </c>
@@ -11335,8 +11838,20 @@
       <c r="F83" s="2">
         <v>0.35110000000000002</v>
       </c>
-    </row>
-    <row r="84" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G83" s="2">
+        <v>0.35110000000000002</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0.35110000000000002</v>
+      </c>
+      <c r="I83" s="2">
+        <v>0.26469999999999999</v>
+      </c>
+      <c r="J83" s="2">
+        <v>-0.20569999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C84" s="1">
         <v>9903</v>
       </c>
@@ -11349,8 +11864,16 @@
       <c r="F84" s="2">
         <v>0.35670000000000002</v>
       </c>
-    </row>
-    <row r="85" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G84" s="2"/>
+      <c r="H84" s="1">
+        <v>0.2041</v>
+      </c>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2">
+        <v>-0.19309999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C85" s="1">
         <v>10711</v>
       </c>
@@ -11363,8 +11886,16 @@
       <c r="F85" s="2">
         <v>0.31909999999999999</v>
       </c>
-    </row>
-    <row r="86" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G85" s="2"/>
+      <c r="H85" s="1">
+        <v>0.19739999999999999</v>
+      </c>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2">
+        <v>-0.27810000000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>9</v>
       </c>
@@ -11380,8 +11911,20 @@
       <c r="F86" s="2">
         <v>0.28270000000000001</v>
       </c>
-    </row>
-    <row r="87" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G86" s="2">
+        <v>0.28270000000000001</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0.2064</v>
+      </c>
+      <c r="I86" s="2">
+        <v>0.18310000000000001</v>
+      </c>
+      <c r="J86" s="2">
+        <v>-0.3604</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C87" s="1">
         <v>11666</v>
       </c>
@@ -11394,8 +11937,16 @@
       <c r="F87" s="2">
         <v>0.34410000000000002</v>
       </c>
-    </row>
-    <row r="88" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G87" s="2"/>
+      <c r="H87" s="1">
+        <v>0.2321</v>
+      </c>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2">
+        <v>-0.22159999999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C88" s="1">
         <v>11503</v>
       </c>
@@ -11408,8 +11959,16 @@
       <c r="F88" s="2">
         <v>0.38300000000000001</v>
       </c>
-    </row>
-    <row r="89" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G88" s="2"/>
+      <c r="H88" s="1">
+        <v>0.25490000000000002</v>
+      </c>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2">
+        <v>-0.13350000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C89" s="1">
         <v>13866</v>
       </c>
@@ -11422,8 +11981,20 @@
       <c r="F89" s="2">
         <v>0.42409999999999998</v>
       </c>
-    </row>
-    <row r="90" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G89" s="2">
+        <v>0.42409999999999998</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0.34079999999999999</v>
+      </c>
+      <c r="I89" s="2">
+        <v>0.3518</v>
+      </c>
+      <c r="J89" s="2">
+        <v>-4.07E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C90" s="1">
         <v>23869</v>
       </c>
@@ -11436,8 +12007,16 @@
       <c r="F90" s="2">
         <v>0.41660000000000003</v>
       </c>
-    </row>
-    <row r="91" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G90" s="2"/>
+      <c r="H90" s="1">
+        <v>0.57750000000000001</v>
+      </c>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2">
+        <v>-5.74E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C91" s="1">
         <v>34912</v>
       </c>
@@ -11450,8 +12029,16 @@
       <c r="F91" s="2">
         <v>0.37090000000000001</v>
       </c>
-    </row>
-    <row r="92" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G91" s="2"/>
+      <c r="H91" s="1">
+        <v>0.75239999999999996</v>
+      </c>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2">
+        <v>-0.16089999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>10</v>
       </c>
@@ -11467,8 +12054,20 @@
       <c r="F92" s="2">
         <v>0.39939999999999998</v>
       </c>
-    </row>
-    <row r="93" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G92" s="2">
+        <v>0.39939999999999998</v>
+      </c>
+      <c r="H92" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I92" s="2">
+        <v>0.32229999999999998</v>
+      </c>
+      <c r="J92" s="2">
+        <v>-9.64E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C93" s="1">
         <v>16657</v>
       </c>
@@ -11481,8 +12080,16 @@
       <c r="F93" s="2">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="94" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G93" s="2"/>
+      <c r="H93" s="1">
+        <v>0.43480000000000002</v>
+      </c>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2">
+        <v>1.7899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C94" s="1">
         <v>11965</v>
       </c>
@@ -11495,8 +12102,16 @@
       <c r="F94" s="2">
         <v>0.41349999999999998</v>
       </c>
-    </row>
-    <row r="95" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G94" s="2"/>
+      <c r="H94" s="1">
+        <v>0.28649999999999998</v>
+      </c>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2">
+        <v>-6.4600000000000005E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C95" s="1">
         <v>8520</v>
       </c>
@@ -11509,8 +12124,20 @@
       <c r="F95" s="2">
         <v>0.496</v>
       </c>
-    </row>
-    <row r="96" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G95" s="2">
+        <v>0.496</v>
+      </c>
+      <c r="H95" s="1">
+        <v>0.2445</v>
+      </c>
+      <c r="I95" s="2">
+        <v>0.43759999999999999</v>
+      </c>
+      <c r="J95" s="2">
+        <v>0.1221</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C96" s="1">
         <v>6397</v>
       </c>
@@ -11523,8 +12150,16 @@
       <c r="F96" s="2">
         <v>0.39500000000000002</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G96" s="2"/>
+      <c r="H96" s="1">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2">
+        <v>-0.10630000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C97" s="1">
         <v>3647</v>
       </c>
@@ -11537,8 +12172,16 @@
       <c r="F97" s="2">
         <v>0.64770000000000005</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G97" s="2"/>
+      <c r="H97" s="1">
+        <v>0.13589999999999999</v>
+      </c>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2">
+        <v>0.4652</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -11557,8 +12200,20 @@
       <c r="F98" s="2">
         <v>0.41930000000000001</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G98" s="2">
+        <v>0.41930000000000001</v>
+      </c>
+      <c r="H98" s="1">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="I98" s="2">
+        <v>0.34610000000000002</v>
+      </c>
+      <c r="J98" s="2">
+        <v>-5.1400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C99" s="1">
         <v>1049</v>
       </c>
@@ -11571,8 +12226,16 @@
       <c r="F99" s="2">
         <v>0.52139999999999997</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G99" s="2"/>
+      <c r="H99" s="1">
+        <v>3.0200000000000001E-2</v>
+      </c>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2">
+        <v>0.1797</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C100" s="1">
         <v>640</v>
       </c>
@@ -11585,8 +12248,16 @@
       <c r="F100" s="2">
         <v>0.52659999999999996</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G100" s="2"/>
+      <c r="H100" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2">
+        <v>0.19120000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C101" s="1">
         <v>268</v>
       </c>
@@ -11599,8 +12270,20 @@
       <c r="F101" s="2">
         <v>0.4627</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G101" s="2">
+        <v>0.4627</v>
+      </c>
+      <c r="H101" s="1">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="I101" s="2">
+        <v>0.39779999999999999</v>
+      </c>
+      <c r="J101" s="2">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C102" s="1">
         <v>327</v>
       </c>
@@ -11613,8 +12296,16 @@
       <c r="F102" s="2">
         <v>0.48620000000000002</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G102" s="2"/>
+      <c r="H102" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C103" s="1">
         <v>1709</v>
       </c>
@@ -11627,8 +12318,16 @@
       <c r="F103" s="2">
         <v>0.34110000000000001</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G103" s="2"/>
+      <c r="H103" s="1">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2">
+        <v>-0.2283</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>8</v>
       </c>
@@ -11644,8 +12343,20 @@
       <c r="F104" s="2">
         <v>0.28029999999999999</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G104" s="2">
+        <v>0.28029999999999999</v>
+      </c>
+      <c r="H104" s="1">
+        <v>9.5600000000000004E-2</v>
+      </c>
+      <c r="I104" s="2">
+        <v>0.1802</v>
+      </c>
+      <c r="J104" s="2">
+        <v>-0.36580000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C105" s="1">
         <v>16401</v>
       </c>
@@ -11658,8 +12369,16 @@
       <c r="F105" s="2">
         <v>0.3417</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G105" s="2"/>
+      <c r="H105" s="1">
+        <v>0.32479999999999998</v>
+      </c>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2">
+        <v>-0.22689999999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C106" s="1">
         <v>29270</v>
       </c>
@@ -11672,8 +12391,16 @@
       <c r="F106" s="2">
         <v>0.39879999999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G106" s="2"/>
+      <c r="H106" s="1">
+        <v>0.67810000000000004</v>
+      </c>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2">
+        <v>-9.7900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C107" s="1">
         <v>16452</v>
       </c>
@@ -11686,8 +12413,20 @@
       <c r="F107" s="2">
         <v>0.42549999999999999</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G107" s="2">
+        <v>0.42549999999999999</v>
+      </c>
+      <c r="H107" s="1">
+        <v>0.40610000000000002</v>
+      </c>
+      <c r="I107" s="2">
+        <v>0.35349999999999998</v>
+      </c>
+      <c r="J107" s="2">
+        <v>-3.73E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C108" s="1">
         <v>10638</v>
       </c>
@@ -11700,8 +12439,16 @@
       <c r="F108" s="2">
         <v>0.40699999999999997</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G108" s="2"/>
+      <c r="H108" s="1">
+        <v>0.2505</v>
+      </c>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2">
+        <v>-7.9200000000000007E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C109" s="1">
         <v>11442</v>
       </c>
@@ -11714,8 +12461,16 @@
       <c r="F109" s="2">
         <v>0.43559999999999999</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G109" s="2"/>
+      <c r="H109" s="1">
+        <v>0.28860000000000002</v>
+      </c>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2">
+        <v>-1.46E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>9</v>
       </c>
@@ -11731,8 +12486,20 @@
       <c r="F110" s="2">
         <v>0.4052</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G110" s="2">
+        <v>0.4052</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0.3216</v>
+      </c>
+      <c r="I110" s="2">
+        <v>0.32919999999999999</v>
+      </c>
+      <c r="J110" s="2">
+        <v>-8.3400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C111" s="1">
         <v>13779</v>
       </c>
@@ -11745,8 +12512,16 @@
       <c r="F111" s="2">
         <v>0.40699999999999997</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G111" s="2"/>
+      <c r="H111" s="1">
+        <v>0.32490000000000002</v>
+      </c>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2">
+        <v>-7.9299999999999995E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C112" s="1">
         <v>14012</v>
       </c>
@@ -11759,8 +12534,16 @@
       <c r="F112" s="2">
         <v>0.37009999999999998</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G112" s="2"/>
+      <c r="H112" s="1">
+        <v>0.3004</v>
+      </c>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2">
+        <v>-0.16270000000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C113" s="1">
         <v>17000</v>
       </c>
@@ -11773,8 +12556,20 @@
       <c r="F113" s="2">
         <v>0.38740000000000002</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G113" s="2">
+        <v>0.38740000000000002</v>
+      </c>
+      <c r="H113" s="1">
+        <v>0.38179999999999997</v>
+      </c>
+      <c r="I113" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="J113" s="2">
+        <v>-0.1237</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C114" s="1">
         <v>26480</v>
       </c>
@@ -11787,8 +12582,16 @@
       <c r="F114" s="2">
         <v>0.30120000000000002</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G114" s="2"/>
+      <c r="H114" s="1">
+        <v>0.46289999999999998</v>
+      </c>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2">
+        <v>-0.31850000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C115" s="1">
         <v>30648</v>
       </c>
@@ -11801,8 +12604,16 @@
       <c r="F115" s="2">
         <v>0.38150000000000001</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G115" s="2"/>
+      <c r="H115" s="1">
+        <v>0.67920000000000003</v>
+      </c>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2">
+        <v>-0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>10</v>
       </c>
@@ -11818,8 +12629,20 @@
       <c r="F116" s="2">
         <v>0.45679999999999998</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G116" s="2">
+        <v>0.45679999999999998</v>
+      </c>
+      <c r="H116" s="1">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="I116" s="2">
+        <v>0.39079999999999998</v>
+      </c>
+      <c r="J116" s="2">
+        <v>3.3399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C117" s="1">
         <v>14436</v>
       </c>
@@ -11832,8 +12655,16 @@
       <c r="F117" s="2">
         <v>0.47389999999999999</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G117" s="2"/>
+      <c r="H117" s="1">
+        <v>0.39679999999999999</v>
+      </c>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2">
+        <v>7.2099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C118" s="1">
         <v>9842</v>
       </c>
@@ -11846,8 +12677,16 @@
       <c r="F118" s="2">
         <v>0.48830000000000001</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G118" s="2"/>
+      <c r="H118" s="1">
+        <v>0.2782</v>
+      </c>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2">
+        <v>0.1047</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C119" s="1">
         <v>7774</v>
       </c>
@@ -11860,8 +12699,20 @@
       <c r="F119" s="2">
         <v>0.40620000000000001</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G119" s="2">
+        <v>0.40620000000000001</v>
+      </c>
+      <c r="H119" s="1">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="I119" s="2">
+        <v>0.33050000000000002</v>
+      </c>
+      <c r="J119" s="2">
+        <v>-8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C120" s="1">
         <v>6617</v>
       </c>
@@ -11874,8 +12725,16 @@
       <c r="F120" s="2">
         <v>0.40960000000000002</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G120" s="2"/>
+      <c r="H120" s="1">
+        <v>0.15620000000000001</v>
+      </c>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2">
+        <v>-7.3499999999999996E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C121" s="1">
         <v>4793</v>
       </c>
@@ -11888,8 +12747,16 @@
       <c r="F121" s="2">
         <v>0.3518</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G121" s="2"/>
+      <c r="H121" s="1">
+        <v>9.6600000000000005E-2</v>
+      </c>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2">
+        <v>-0.20419999999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>16</v>
       </c>
@@ -11908,8 +12775,20 @@
       <c r="F122" s="2">
         <v>0.44519999999999998</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G122" s="2">
+        <v>0.44519999999999998</v>
+      </c>
+      <c r="H122" s="1">
+        <v>8.2100000000000006E-2</v>
+      </c>
+      <c r="I122" s="2">
+        <v>0.377</v>
+      </c>
+      <c r="J122" s="2">
+        <v>7.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C123" s="1">
         <v>2516</v>
       </c>
@@ -11922,8 +12801,16 @@
       <c r="F123" s="2">
         <v>0.4909</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G123" s="2"/>
+      <c r="H123" s="1">
+        <v>7.0300000000000001E-2</v>
+      </c>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2">
+        <v>0.1105</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C124" s="1">
         <v>1741</v>
       </c>
@@ -11936,8 +12823,16 @@
       <c r="F124" s="2">
         <v>0.3538</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G124" s="2"/>
+      <c r="H124" s="1">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2">
+        <v>-0.1996</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C125" s="1">
         <v>586</v>
       </c>
@@ -11950,8 +12845,20 @@
       <c r="F125" s="2">
         <v>0.36009999999999998</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G125" s="2">
+        <v>0.36009999999999998</v>
+      </c>
+      <c r="H125" s="1">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="I125" s="2">
+        <v>0.27539999999999998</v>
+      </c>
+      <c r="J125" s="2">
+        <v>-0.18540000000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C126" s="1">
         <v>367</v>
       </c>
@@ -11964,8 +12871,16 @@
       <c r="F126" s="2">
         <v>0.248</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G126" s="2"/>
+      <c r="H126" s="1">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="I126" s="2"/>
+      <c r="J126" s="2">
+        <v>-0.43909999999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C127" s="1">
         <v>481</v>
       </c>
@@ -11978,8 +12893,16 @@
       <c r="F127" s="2">
         <v>0.58420000000000005</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G127" s="2"/>
+      <c r="H127" s="1">
+        <v>1.47E-2</v>
+      </c>
+      <c r="I127" s="2"/>
+      <c r="J127" s="2">
+        <v>0.3216</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>8</v>
       </c>
@@ -11995,8 +12918,20 @@
       <c r="F128" s="2">
         <v>0.42730000000000001</v>
       </c>
-    </row>
-    <row r="129" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G128" s="2">
+        <v>0.42730000000000001</v>
+      </c>
+      <c r="H128" s="1">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="I128" s="2">
+        <v>0.35560000000000003</v>
+      </c>
+      <c r="J128" s="2">
+        <v>-3.3300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C129" s="1">
         <v>2891</v>
       </c>
@@ -12009,8 +12944,16 @@
       <c r="F129" s="2">
         <v>0.35039999999999999</v>
       </c>
-    </row>
-    <row r="130" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G129" s="2"/>
+      <c r="H129" s="1">
+        <v>5.74E-2</v>
+      </c>
+      <c r="I129" s="2"/>
+      <c r="J129" s="2">
+        <v>-0.20730000000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C130" s="1">
         <v>5710</v>
       </c>
@@ -12023,8 +12966,16 @@
       <c r="F130" s="2">
         <v>0.40960000000000002</v>
       </c>
-    </row>
-    <row r="131" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G130" s="2"/>
+      <c r="H130" s="1">
+        <v>0.1346</v>
+      </c>
+      <c r="I130" s="2"/>
+      <c r="J130" s="2">
+        <v>-7.3300000000000004E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C131" s="1">
         <v>8861</v>
       </c>
@@ -12037,8 +12988,20 @@
       <c r="F131" s="2">
         <v>0.46200000000000002</v>
       </c>
-    </row>
-    <row r="132" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G131" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="H131" s="1">
+        <v>0.23680000000000001</v>
+      </c>
+      <c r="I131" s="2">
+        <v>0.39710000000000001</v>
+      </c>
+      <c r="J131" s="2">
+        <v>4.5199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C132" s="1">
         <v>12208</v>
       </c>
@@ -12051,8 +13014,16 @@
       <c r="F132" s="2">
         <v>0.44540000000000002</v>
       </c>
-    </row>
-    <row r="133" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G132" s="2"/>
+      <c r="H132" s="1">
+        <v>0.315</v>
+      </c>
+      <c r="I132" s="2"/>
+      <c r="J132" s="2">
+        <v>7.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C133" s="1">
         <v>14567</v>
       </c>
@@ -12065,8 +13036,16 @@
       <c r="F133" s="2">
         <v>0.54139999999999999</v>
       </c>
-    </row>
-    <row r="134" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G133" s="2"/>
+      <c r="H133" s="1">
+        <v>0.4577</v>
+      </c>
+      <c r="I133" s="2"/>
+      <c r="J133" s="2">
+        <v>0.22489999999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>9</v>
       </c>
@@ -12082,8 +13061,20 @@
       <c r="F134" s="2">
         <v>0.59419999999999995</v>
       </c>
-    </row>
-    <row r="135" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G134" s="2">
+        <v>0.59419999999999995</v>
+      </c>
+      <c r="H134" s="1">
+        <v>0.56469999999999998</v>
+      </c>
+      <c r="I134" s="2">
+        <v>0.55479999999999996</v>
+      </c>
+      <c r="J134" s="2">
+        <v>0.34420000000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C135" s="1">
         <v>17361</v>
       </c>
@@ -12096,8 +13087,16 @@
       <c r="F135" s="2">
         <v>0.54600000000000004</v>
       </c>
-    </row>
-    <row r="136" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G135" s="2"/>
+      <c r="H135" s="1">
+        <v>0.5504</v>
+      </c>
+      <c r="I135" s="2"/>
+      <c r="J135" s="2">
+        <v>0.23519999999999999</v>
+      </c>
+    </row>
+    <row r="136" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C136" s="1">
         <v>17344</v>
       </c>
@@ -12110,8 +13109,16 @@
       <c r="F136" s="2">
         <v>0.56430000000000002</v>
       </c>
-    </row>
-    <row r="137" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G136" s="2"/>
+      <c r="H136" s="1">
+        <v>0.56840000000000002</v>
+      </c>
+      <c r="I136" s="2"/>
+      <c r="J136" s="2">
+        <v>0.2767</v>
+      </c>
+    </row>
+    <row r="137" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C137" s="1">
         <v>17341</v>
       </c>
@@ -12124,8 +13131,20 @@
       <c r="F137" s="2">
         <v>0.58169999999999999</v>
       </c>
-    </row>
-    <row r="138" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G137" s="2">
+        <v>0.58169999999999999</v>
+      </c>
+      <c r="H137" s="1">
+        <v>0.58579999999999999</v>
+      </c>
+      <c r="I137" s="2">
+        <v>0.53979999999999995</v>
+      </c>
+      <c r="J137" s="2">
+        <v>0.31590000000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C138" s="1">
         <v>17214</v>
       </c>
@@ -12138,8 +13157,16 @@
       <c r="F138" s="2">
         <v>0.53639999999999999</v>
       </c>
-    </row>
-    <row r="139" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G138" s="2"/>
+      <c r="H138" s="1">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="I138" s="2"/>
+      <c r="J138" s="2">
+        <v>0.21340000000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C139" s="1">
         <v>16116</v>
       </c>
@@ -12152,8 +13179,16 @@
       <c r="F139" s="2">
         <v>0.55110000000000003</v>
       </c>
-    </row>
-    <row r="140" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G139" s="2"/>
+      <c r="H139" s="1">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="I139" s="2"/>
+      <c r="J139" s="2">
+        <v>0.2467</v>
+      </c>
+    </row>
+    <row r="140" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>10</v>
       </c>
@@ -12169,8 +13204,20 @@
       <c r="F140" s="2">
         <v>0.5595</v>
       </c>
-    </row>
-    <row r="141" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G140" s="2">
+        <v>0.5595</v>
+      </c>
+      <c r="H140" s="1">
+        <v>0.46989999999999998</v>
+      </c>
+      <c r="I140" s="2">
+        <v>0.51339999999999997</v>
+      </c>
+      <c r="J140" s="2">
+        <v>0.26579999999999998</v>
+      </c>
+    </row>
+    <row r="141" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C141" s="1">
         <v>11797</v>
       </c>
@@ -12183,8 +13230,16 @@
       <c r="F141" s="2">
         <v>0.54059999999999997</v>
       </c>
-    </row>
-    <row r="142" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G141" s="2"/>
+      <c r="H141" s="1">
+        <v>0.36980000000000002</v>
+      </c>
+      <c r="I141" s="2"/>
+      <c r="J141" s="2">
+        <v>0.22309999999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C142" s="1">
         <v>8657</v>
       </c>
@@ -12197,8 +13252,16 @@
       <c r="F142" s="2">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="143" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G142" s="2"/>
+      <c r="H142" s="1">
+        <v>0.26050000000000001</v>
+      </c>
+      <c r="I142" s="2"/>
+      <c r="J142" s="2">
+        <v>0.17649999999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C143" s="1">
         <v>6888</v>
       </c>
@@ -12211,8 +13274,20 @@
       <c r="F143" s="2">
         <v>0.58260000000000001</v>
       </c>
-    </row>
-    <row r="144" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G143" s="2">
+        <v>0.58260000000000001</v>
+      </c>
+      <c r="H143" s="1">
+        <v>0.2321</v>
+      </c>
+      <c r="I143" s="2">
+        <v>0.54090000000000005</v>
+      </c>
+      <c r="J143" s="2">
+        <v>0.318</v>
+      </c>
+    </row>
+    <row r="144" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C144" s="1">
         <v>5918</v>
       </c>
@@ -12225,8 +13300,16 @@
       <c r="F144" s="2">
         <v>0.53080000000000005</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G144" s="2"/>
+      <c r="H144" s="1">
+        <v>0.18129999999999999</v>
+      </c>
+      <c r="I144" s="2"/>
+      <c r="J144" s="2">
+        <v>0.20069999999999999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C145" s="1">
         <v>4377</v>
       </c>
@@ -12239,8 +13322,16 @@
       <c r="F145" s="2">
         <v>0.55469999999999997</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G145" s="2"/>
+      <c r="H145" s="1">
+        <v>0.13980000000000001</v>
+      </c>
+      <c r="I145" s="2"/>
+      <c r="J145" s="2">
+        <v>0.25490000000000002</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>17</v>
       </c>
@@ -12259,8 +13350,20 @@
       <c r="F146" s="2">
         <v>0.58389999999999997</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G146" s="2">
+        <v>0.58389999999999997</v>
+      </c>
+      <c r="H146" s="1">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="I146" s="2">
+        <v>0.54249999999999998</v>
+      </c>
+      <c r="J146" s="2">
+        <v>0.32100000000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C147" s="1">
         <v>2785</v>
       </c>
@@ -12273,8 +13376,16 @@
       <c r="F147" s="2">
         <v>0.70230000000000004</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G147" s="2"/>
+      <c r="H147" s="1">
+        <v>0.1123</v>
+      </c>
+      <c r="I147" s="2"/>
+      <c r="J147" s="2">
+        <v>0.58889999999999998</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C148" s="1">
         <v>1943</v>
       </c>
@@ -12287,8 +13398,16 @@
       <c r="F148" s="2">
         <v>0.52080000000000004</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G148" s="2"/>
+      <c r="H148" s="1">
+        <v>5.7299999999999997E-2</v>
+      </c>
+      <c r="I148" s="2"/>
+      <c r="J148" s="2">
+        <v>0.17829999999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C149" s="1">
         <v>571</v>
       </c>
@@ -12301,8 +13420,20 @@
       <c r="F149" s="2">
         <v>0.38879999999999998</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G149" s="2">
+        <v>0.38879999999999998</v>
+      </c>
+      <c r="H149" s="1">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="I149" s="2">
+        <v>0.30969999999999998</v>
+      </c>
+      <c r="J149" s="2">
+        <v>-0.12039999999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C150" s="1">
         <v>268</v>
       </c>
@@ -12315,8 +13446,16 @@
       <c r="F150" s="2">
         <v>0.73129999999999995</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G150" s="2"/>
+      <c r="H150" s="1">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="I150" s="2"/>
+      <c r="J150" s="2">
+        <v>0.65449999999999997</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C151" s="1">
         <v>421</v>
       </c>
@@ -12329,8 +13468,16 @@
       <c r="F151" s="2">
         <v>0.74819999999999998</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G151" s="2"/>
+      <c r="H151" s="1">
+        <v>1.67E-2</v>
+      </c>
+      <c r="I151" s="2"/>
+      <c r="J151" s="2">
+        <v>0.69269999999999998</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>8</v>
       </c>
@@ -12346,8 +13493,20 @@
       <c r="F152" s="2">
         <v>0.68389999999999995</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G152" s="2">
+        <v>0.68389999999999995</v>
+      </c>
+      <c r="H152" s="1">
+        <v>3.4599999999999999E-2</v>
+      </c>
+      <c r="I152" s="2">
+        <v>0.66180000000000005</v>
+      </c>
+      <c r="J152" s="2">
+        <v>0.54710000000000003</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C153" s="1">
         <v>1935</v>
       </c>
@@ -12360,8 +13519,16 @@
       <c r="F153" s="2">
         <v>0.56489999999999996</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G153" s="2"/>
+      <c r="H153" s="1">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I153" s="2"/>
+      <c r="J153" s="2">
+        <v>0.27789999999999998</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C154" s="1">
         <v>4500</v>
       </c>
@@ -12374,8 +13541,16 @@
       <c r="F154" s="2">
         <v>0.58420000000000005</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G154" s="2"/>
+      <c r="H154" s="1">
+        <v>0.1515</v>
+      </c>
+      <c r="I154" s="2"/>
+      <c r="J154" s="2">
+        <v>0.32169999999999999</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C155" s="1">
         <v>7620</v>
       </c>
@@ -12388,8 +13563,20 @@
       <c r="F155" s="2">
         <v>0.57940000000000003</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G155" s="2">
+        <v>0.57940000000000003</v>
+      </c>
+      <c r="H155" s="1">
+        <v>0.2555</v>
+      </c>
+      <c r="I155" s="2">
+        <v>0.53710000000000002</v>
+      </c>
+      <c r="J155" s="2">
+        <v>0.31080000000000002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C156" s="1">
         <v>11093</v>
       </c>
@@ -12402,8 +13589,16 @@
       <c r="F156" s="2">
         <v>0.51719999999999999</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G156" s="2"/>
+      <c r="H156" s="1">
+        <v>0.33250000000000002</v>
+      </c>
+      <c r="I156" s="2"/>
+      <c r="J156" s="2">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C157" s="1">
         <v>13401</v>
       </c>
@@ -12416,8 +13611,16 @@
       <c r="F157" s="2">
         <v>0.50290000000000001</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G157" s="2"/>
+      <c r="H157" s="1">
+        <v>0.39079999999999998</v>
+      </c>
+      <c r="I157" s="2"/>
+      <c r="J157" s="2">
+        <v>0.1376</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>9</v>
       </c>
@@ -12433,8 +13636,20 @@
       <c r="F158" s="2">
         <v>0.45829999999999999</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G158" s="2">
+        <v>0.45829999999999999</v>
+      </c>
+      <c r="H158" s="1">
+        <v>0.41589999999999999</v>
+      </c>
+      <c r="I158" s="2">
+        <v>0.3926</v>
+      </c>
+      <c r="J158" s="2">
+        <v>3.6700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C159" s="1">
         <v>16761</v>
       </c>
@@ -12447,8 +13662,16 @@
       <c r="F159" s="2">
         <v>0.4531</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G159" s="2"/>
+      <c r="H159" s="1">
+        <v>0.44069999999999998</v>
+      </c>
+      <c r="I159" s="2"/>
+      <c r="J159" s="2">
+        <v>2.5100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C160" s="1">
         <v>16736</v>
       </c>
@@ -12461,8 +13684,16 @@
       <c r="F160" s="2">
         <v>0.42930000000000001</v>
       </c>
-    </row>
-    <row r="161" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G160" s="2"/>
+      <c r="H160" s="1">
+        <v>0.41670000000000001</v>
+      </c>
+      <c r="I160" s="2"/>
+      <c r="J160" s="2">
+        <v>-2.8899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C161" s="1">
         <v>16848</v>
       </c>
@@ -12475,8 +13706,20 @@
       <c r="F161" s="2">
         <v>0.40560000000000002</v>
       </c>
-    </row>
-    <row r="162" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G161" s="2">
+        <v>0.40560000000000002</v>
+      </c>
+      <c r="H161" s="1">
+        <v>0.39629999999999999</v>
+      </c>
+      <c r="I161" s="2">
+        <v>0.32979999999999998</v>
+      </c>
+      <c r="J161" s="2">
+        <v>-8.2400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C162" s="1">
         <v>16426</v>
       </c>
@@ -12489,8 +13732,16 @@
       <c r="F162" s="2">
         <v>0.46550000000000002</v>
       </c>
-    </row>
-    <row r="163" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G162" s="2"/>
+      <c r="H162" s="1">
+        <v>0.44369999999999998</v>
+      </c>
+      <c r="I162" s="2"/>
+      <c r="J162" s="2">
+        <v>5.3199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C163" s="1">
         <v>15527</v>
       </c>
@@ -12503,8 +13754,16 @@
       <c r="F163" s="2">
         <v>0.4723</v>
       </c>
-    </row>
-    <row r="164" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G163" s="2"/>
+      <c r="H163" s="1">
+        <v>0.4254</v>
+      </c>
+      <c r="I163" s="2"/>
+      <c r="J163" s="2">
+        <v>6.8400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>10</v>
       </c>
@@ -12520,8 +13779,20 @@
       <c r="F164" s="2">
         <v>0.51100000000000001</v>
       </c>
-    </row>
-    <row r="165" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G164" s="2">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="H164" s="1">
+        <v>0.40839999999999999</v>
+      </c>
+      <c r="I164" s="2">
+        <v>0.45540000000000003</v>
+      </c>
+      <c r="J164" s="2">
+        <v>0.15590000000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C165" s="1">
         <v>10698</v>
       </c>
@@ -12534,8 +13805,16 @@
       <c r="F165" s="2">
         <v>0.4743</v>
       </c>
-    </row>
-    <row r="166" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G165" s="2"/>
+      <c r="H165" s="1">
+        <v>0.29389999999999999</v>
+      </c>
+      <c r="I165" s="2"/>
+      <c r="J165" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C166" s="1">
         <v>7506</v>
       </c>
@@ -12548,8 +13827,16 @@
       <c r="F166" s="2">
         <v>0.59989999999999999</v>
       </c>
-    </row>
-    <row r="167" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G166" s="2"/>
+      <c r="H166" s="1">
+        <v>0.2606</v>
+      </c>
+      <c r="I166" s="2"/>
+      <c r="J166" s="2">
+        <v>0.35720000000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C167" s="1">
         <v>5498</v>
       </c>
@@ -12562,8 +13849,20 @@
       <c r="F167" s="2">
         <v>0.53869999999999996</v>
       </c>
-    </row>
-    <row r="168" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G167" s="2">
+        <v>0.53869999999999996</v>
+      </c>
+      <c r="H167" s="1">
+        <v>0.1709</v>
+      </c>
+      <c r="I167" s="2">
+        <v>0.48859999999999998</v>
+      </c>
+      <c r="J167" s="2">
+        <v>0.21879999999999999</v>
+      </c>
+    </row>
+    <row r="168" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C168" s="1">
         <v>4043</v>
       </c>
@@ -12576,8 +13875,16 @@
       <c r="F168" s="2">
         <v>0.62380000000000002</v>
       </c>
-    </row>
-    <row r="169" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G168" s="2"/>
+      <c r="H168" s="1">
+        <v>0.1452</v>
+      </c>
+      <c r="I168" s="2"/>
+      <c r="J168" s="2">
+        <v>0.41120000000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>11</v>
       </c>
@@ -12592,6 +13899,18 @@
       </c>
       <c r="F169" s="2">
         <v>0.50039999999999996</v>
+      </c>
+      <c r="G169" s="2">
+        <v>0.50039999999999996</v>
+      </c>
+      <c r="H169" s="1">
+        <v>8.14E-2</v>
+      </c>
+      <c r="I169" s="2">
+        <v>0.44280000000000003</v>
+      </c>
+      <c r="J169" s="2">
+        <v>0.13189999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -12604,7 +13923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0C4562-A8B8-414D-8141-9EE817B47AF2}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -12993,7 +14312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA64C4F-F537-6240-8362-0F566F7307B7}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>

</xml_diff>